<commit_message>
Endosos para polizas blanket y complementaria
</commit_message>
<xml_diff>
--- a/Sura/EmisionMotor_PolizaBlanket.xlsx
+++ b/Sura/EmisionMotor_PolizaBlanket.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMP\Polizas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE271891-22BD-499F-BAB6-1E8FF3834326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039B7082-DCE8-4BDA-BAFD-155505CCFEE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F27E0E3-BF46-4A34-AA48-A046ADCD8784}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Ambiente</t>
   </si>
@@ -105,10 +105,16 @@
     <t>No</t>
   </si>
   <si>
-    <t>14/01/2021</t>
-  </si>
-  <si>
     <t>Kms</t>
+  </si>
+  <si>
+    <t>CodigoAgente</t>
+  </si>
+  <si>
+    <t>NUM_GRUPO</t>
+  </si>
+  <si>
+    <t>Corporativos Directos</t>
   </si>
 </sst>
 </file>
@@ -479,15 +485,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4C55B-7E7D-457C-AD66-64215B360016}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,49 +507,55 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>27</v>
+      <c r="T1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -556,33 +568,37 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
+        <v>6965</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3">
         <v>3942691124</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2">
-        <v>1000</v>
-      </c>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2">
+        <v>2500</v>
+      </c>
       <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>